<commit_message>
resolucion de paradasTransporte y agregado de funcion de calcular distancia dentro de la interfaz transporte
</commit_message>
<xml_diff>
--- a/src/main/resources/files/tablaTest.xlsx
+++ b/src/main/resources/files/tablaTest.xlsx
@@ -69,6 +69,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +390,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,9 +440,7 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2">
-        <v>44785</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -452,9 +453,7 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2">
-        <v>44784</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -469,9 +468,7 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2">
-        <v>44783</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -482,5 +479,6 @@
     <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementacion calculoDistancia en tramos y trayectos
</commit_message>
<xml_diff>
--- a/src/main/resources/files/tablaTest.xlsx
+++ b/src/main/resources/files/tablaTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Actividad</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">Combustible consumido - Gasoil </t>
+  </si>
+  <si>
+    <t>SS</t>
   </si>
 </sst>
 </file>
@@ -70,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -103,10 +106,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,34 +404,34 @@
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -440,10 +443,12 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="E3" s="1">
+        <v>44784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -453,9 +458,11 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>44784</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -468,7 +475,14 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="1">
+        <v>44784</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
no se subieron los cambios lcdll
</commit_message>
<xml_diff>
--- a/src/main/resources/files/tablaTest.xlsx
+++ b/src/main/resources/files/tablaTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Actividad</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t xml:space="preserve">Combustible consumido - Gasoil </t>
-  </si>
-  <si>
-    <t>SS</t>
   </si>
 </sst>
 </file>
@@ -390,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +401,7 @@
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -419,7 +416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" t="s">
@@ -430,7 +427,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -447,7 +444,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>10</v>
@@ -462,7 +459,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -477,11 +474,6 @@
       </c>
       <c r="E5" s="1">
         <v>44784</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Termino el switch del lectorExcel
</commit_message>
<xml_diff>
--- a/src/main/resources/files/tablaTest.xlsx
+++ b/src/main/resources/files/tablaTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Actividad</t>
   </si>
@@ -101,12 +101,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +391,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +429,7 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -445,7 +446,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -477,12 +480,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Agrego test calculo huella
</commit_message>
<xml_diff>
--- a/src/main/resources/files/tablaTest.xlsx
+++ b/src/main/resources/files/tablaTest.xlsx
@@ -62,7 +62,7 @@
     <t>Anual</t>
   </si>
   <si>
-    <t xml:space="preserve">Combustible consumido - Gasoil </t>
+    <t>Gasoil</t>
   </si>
 </sst>
 </file>
@@ -104,10 +104,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,33 +403,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -446,7 +446,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">

</xml_diff>